<commit_message>
Update CSDID Effect Estimate.xlsx
</commit_message>
<xml_diff>
--- a/Output/CSDID Effect Estimate.xlsx
+++ b/Output/CSDID Effect Estimate.xlsx
@@ -1,152 +1,139 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benjamin Glasner\EIG Dropbox\Benjamin Glasner\EIG\HUD Agg USPS Administrative Data on Vacancies\output\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C538864E-0E7C-4494-A23A-0EC0D90374D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
-  <si>
-    <t>Tract Geography</t>
-  </si>
-  <si>
-    <t>Active and Vacant Residential</t>
-  </si>
-  <si>
-    <t>Log(Active and Vacant Residential)</t>
-  </si>
-  <si>
-    <t>Active Residential</t>
-  </si>
-  <si>
-    <t>Log(Active Residential)</t>
-  </si>
-  <si>
-    <t>All</t>
-  </si>
-  <si>
-    <t>Large urban</t>
-  </si>
-  <si>
-    <t>Mid-sized urban</t>
-  </si>
-  <si>
-    <t>0.0286  (0.0137)</t>
-  </si>
-  <si>
-    <t>Small urban</t>
-  </si>
-  <si>
-    <t>Suburban</t>
-  </si>
-  <si>
-    <t>Small town</t>
-  </si>
-  <si>
-    <t>0.0122  (0.006)</t>
-  </si>
-  <si>
-    <t>15.76  (5.85)</t>
-  </si>
-  <si>
-    <t>Rural</t>
-  </si>
-  <si>
-    <t>19.13  (7.52)</t>
-  </si>
-  <si>
-    <t>0.0063  (0.0044)</t>
-  </si>
-  <si>
-    <t>11.93  (6.98)</t>
-  </si>
-  <si>
-    <t>16.61 ** (5.74)</t>
-  </si>
-  <si>
-    <t>0.0178 ** (0.0055)</t>
-  </si>
-  <si>
-    <t>35.66 *** (3.06)</t>
-  </si>
-  <si>
-    <t>49.74 *** (5.55)</t>
-  </si>
-  <si>
-    <t>58.85 *** (9.56)</t>
-  </si>
-  <si>
-    <t>33.49 *** (6.23)</t>
-  </si>
-  <si>
-    <t>38.15 *** (7.96)</t>
-  </si>
-  <si>
-    <t>0.0211 *** (0.0021)</t>
-  </si>
-  <si>
-    <t>0.0357 *** (0.0041)</t>
-  </si>
-  <si>
-    <t>0.0213 *** (0.0045)</t>
-  </si>
-  <si>
-    <t>31.94 *** (2.88)</t>
-  </si>
-  <si>
-    <t>43.53 *** (5.57)</t>
-  </si>
-  <si>
-    <t>53.3 *** (9.88)</t>
-  </si>
-  <si>
-    <t>28.06 *** (6.2)</t>
-  </si>
-  <si>
-    <t>34.52 *** (8.13)</t>
-  </si>
-  <si>
-    <t>0.0191 *** (0.0024)</t>
-  </si>
-  <si>
-    <t>0.0312 *** (0.0043)</t>
-  </si>
-  <si>
-    <t>0.0235  (0.0142)</t>
-  </si>
-  <si>
-    <t>0.0204 *** (0.004)</t>
-  </si>
-  <si>
-    <t>0.0162  (0.0059)</t>
-  </si>
-  <si>
-    <t>0.0132  (0.0058)</t>
-  </si>
-  <si>
-    <t>0.0011 ** (0.0041)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+  <si>
+    <t xml:space="preserve">Tract Geography</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Active and Vacant Residential</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log(Active and Vacant Residential)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Active Residential</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log(Active Residential)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35.68 * (2.78)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0205 * (0.0019)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31.96 * (2.86)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.02 * (0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Large urban</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49.73 * (5.67)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0345 * (0.0037)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43.52 * (5.61)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.03 * (0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mid-sized urban</t>
+  </si>
+  <si>
+    <t xml:space="preserve">59 * (11.25)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0288  (0.0135)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">53.45 * (10.48)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.02  (0.01)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Small urban</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33.52 * (6.39)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0215 * (0.0039)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28.09 * (6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suburban</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38.05 * (7.83)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0163  (0.0049)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34.37 * (7.59)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.01  (0.01)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Small town</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16.59  (5.86)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0117  (0.0059)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15.72  (5.75)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rural</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.18  (7.23)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0068  (0.0046)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.99  (6.94)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 * (0)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -182,15 +169,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -472,22 +450,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -504,127 +474,127 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
         <v>25</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
         <v>28</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="B8" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="C8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="D8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="E8" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>